<commit_message>
Replaces Avij vars with Avii' vars in month model
</commit_message>
<xml_diff>
--- a/Code/Overlap/RowCol calc.xlsx
+++ b/Code/Overlap/RowCol calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Code\Overlap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC056D56-D6D8-4F06-8B60-72D38D945E89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AFB3EC-7247-4D37-A3CF-821CF9A7D25B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F85780C8-78EB-42E2-BE9E-CEC15D110F12}"/>
+    <workbookView xWindow="28680" yWindow="840" windowWidth="19440" windowHeight="15000" xr2:uid="{F85780C8-78EB-42E2-BE9E-CEC15D110F12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Rows</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Limit2</t>
+  </si>
+  <si>
+    <t>aL</t>
+  </si>
+  <si>
+    <t>aF</t>
   </si>
 </sst>
 </file>
@@ -445,39 +451,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369586FE-FB47-484D-B8DA-5DFCD0818EDC}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9:M30"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -485,108 +491,179 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <f>B3+B4</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11">
         <f>SUM(B12:B18)</f>
-        <v>1511</v>
+        <v>15819</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E11">
         <f>SUM(E12:E18)</f>
-        <v>6516</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>67194</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f>SUM(H12:H17)</f>
+        <v>1029</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <f>SUM(K12:K17)</f>
+        <v>5742</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12">
         <f>B2*B3</f>
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D12">
         <f>B5</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E12">
         <f>B12*D12</f>
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>972</v>
+      </c>
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <f>B2</f>
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <f>B5</f>
+        <v>18</v>
+      </c>
+      <c r="K12">
+        <f>H12*J12</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13">
         <f>B2*B5</f>
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="D13">
         <f>B5</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E13">
         <f t="shared" ref="E13:E18" si="0">B13*D13</f>
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>972</v>
+      </c>
+      <c r="G13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <f>B2*B5</f>
+        <v>54</v>
+      </c>
+      <c r="J13">
+        <f>2+2*(B5-1)</f>
+        <v>36</v>
+      </c>
+      <c r="K13">
+        <f>H13*J13</f>
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="B14">
         <f>B2*(B3-1)</f>
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <f>2*B5</f>
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>264</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1836</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14">
+        <f>B1*B3</f>
+        <v>36</v>
+      </c>
+      <c r="J14">
+        <f>(B2/B1)*B5</f>
+        <v>27</v>
+      </c>
+      <c r="K14">
+        <f>H14*J14</f>
+        <v>972</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15">
         <f>B1*B3</f>
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="D15">
         <f>B2/B1 * B5</f>
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>972</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15">
+        <f>B2*B5*(B5-1)</f>
+        <v>918</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <f>H15*J15</f>
+        <v>2754</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
       <c r="B16">
         <f>B2*B5*(B5-1)*(B5-1)</f>
-        <v>1452</v>
+        <v>15606</v>
       </c>
       <c r="D16">
         <f>4</f>
@@ -594,26 +671,55 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>5808</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>62424</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <f>B3</f>
+        <v>18</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <f>H16*J16</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
       <c r="B17">
         <f>B3</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17">
+        <f>B4*B2</f>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f>B5</f>
+        <v>18</v>
+      </c>
+      <c r="K17">
+        <f>H17*J17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
@@ -623,40 +729,77 @@
       </c>
       <c r="D18">
         <f>B5</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <f>H20+H21+H22+H23</f>
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B20">
         <f>B21+B22</f>
-        <v>156</v>
-      </c>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>990</v>
+      </c>
+      <c r="G20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20">
+        <f>B5</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
       <c r="B21">
         <f>B3</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21">
+        <f>B2*B5*B5</f>
+        <v>972</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
       <c r="B22">
         <f>B2*B3*B3</f>
-        <v>144</v>
+        <v>972</v>
+      </c>
+      <c r="G22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22">
+        <f>B2*B5</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23">
+        <f>B2*B5</f>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change Avij vars in code
</commit_message>
<xml_diff>
--- a/Code/Overlap/RowCol calc.xlsx
+++ b/Code/Overlap/RowCol calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Code\Overlap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AFB3EC-7247-4D37-A3CF-821CF9A7D25B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4580CF07-10AC-4AE5-B3A9-4DB6E080819E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="840" windowWidth="19440" windowHeight="15000" xr2:uid="{F85780C8-78EB-42E2-BE9E-CEC15D110F12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F85780C8-78EB-42E2-BE9E-CEC15D110F12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +464,7 @@
         <v>2</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -472,7 +472,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -480,7 +480,7 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -497,7 +497,7 @@
       </c>
       <c r="B5">
         <f>B3+B4</f>
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -506,28 +506,28 @@
       </c>
       <c r="B11">
         <f>SUM(B12:B18)</f>
-        <v>15819</v>
+        <v>2435</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E11">
         <f>SUM(E12:E18)</f>
-        <v>67194</v>
+        <v>10430</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H11">
         <f>SUM(H12:H17)</f>
-        <v>1029</v>
+        <v>225</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K11">
         <f>SUM(K12:K17)</f>
-        <v>5742</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -536,30 +536,30 @@
       </c>
       <c r="B12">
         <f>B2*B3</f>
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="D12">
         <f>B5</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E12">
         <f>B12*D12</f>
-        <v>972</v>
+        <v>196</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
       </c>
       <c r="H12">
         <f>B2</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J12">
         <f>B5</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K12">
-        <f>H12*J12</f>
-        <v>54</v>
+        <f t="shared" ref="K12:K17" si="0">H12*J12</f>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -568,30 +568,30 @@
       </c>
       <c r="B13">
         <f>B2*B5</f>
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="D13">
         <f>B5</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="E13:E18" si="0">B13*D13</f>
-        <v>972</v>
+        <f t="shared" ref="E13:E18" si="1">B13*D13</f>
+        <v>196</v>
       </c>
       <c r="G13" t="s">
         <v>7</v>
       </c>
       <c r="H13">
         <f>B2*B5</f>
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="J13">
         <f>2+2*(B5-1)</f>
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="K13">
-        <f>H13*J13</f>
-        <v>1944</v>
+        <f t="shared" si="0"/>
+        <v>392</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -600,30 +600,30 @@
       </c>
       <c r="B14">
         <f>B2*(B3-1)</f>
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="D14">
         <f>2*B5</f>
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>1836</v>
+        <f t="shared" si="1"/>
+        <v>364</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
       </c>
       <c r="H14">
         <f>B1*B3</f>
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="J14">
         <f>(B2/B1)*B5</f>
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="K14">
-        <f>H14*J14</f>
-        <v>972</v>
+        <f t="shared" si="0"/>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -632,29 +632,29 @@
       </c>
       <c r="B15">
         <f>B1*B3</f>
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D15">
         <f>B2/B1 * B5</f>
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>972</v>
+        <f t="shared" si="1"/>
+        <v>196</v>
       </c>
       <c r="G15" t="s">
         <v>9</v>
       </c>
       <c r="H15">
         <f>B2*B5*(B5-1)</f>
-        <v>918</v>
+        <v>182</v>
       </c>
       <c r="J15">
         <v>3</v>
       </c>
       <c r="K15">
-        <f>H15*J15</f>
-        <v>2754</v>
+        <f t="shared" si="0"/>
+        <v>546</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -663,29 +663,29 @@
       </c>
       <c r="B16">
         <f>B2*B5*(B5-1)*(B5-1)</f>
-        <v>15606</v>
+        <v>2366</v>
       </c>
       <c r="D16">
         <f>4</f>
         <v>4</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>62424</v>
+        <f t="shared" si="1"/>
+        <v>9464</v>
       </c>
       <c r="G16" t="s">
         <v>10</v>
       </c>
       <c r="H16">
         <f>B3</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J16">
         <v>1</v>
       </c>
       <c r="K16">
-        <f>H16*J16</f>
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -694,14 +694,14 @@
       </c>
       <c r="B17">
         <f>B3</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>11</v>
@@ -712,10 +712,10 @@
       </c>
       <c r="J17">
         <f>B5</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K17">
-        <f>H17*J17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -729,10 +729,10 @@
       </c>
       <c r="D18">
         <f>B5</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -742,7 +742,7 @@
       </c>
       <c r="H19">
         <f>H20+H21+H22+H23</f>
-        <v>1098</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -751,14 +751,14 @@
       </c>
       <c r="B20">
         <f>B21+B22</f>
-        <v>990</v>
+        <v>210</v>
       </c>
       <c r="G20" t="s">
         <v>12</v>
       </c>
       <c r="H20">
         <f>B5</f>
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -767,14 +767,14 @@
       </c>
       <c r="B21">
         <f>B3</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G21" t="s">
         <v>13</v>
       </c>
       <c r="H21">
-        <f>B2*B5*B5</f>
-        <v>972</v>
+        <f>B2*B5*(B5-1)</f>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -783,14 +783,14 @@
       </c>
       <c r="B22">
         <f>B2*B3*B3</f>
-        <v>972</v>
+        <v>196</v>
       </c>
       <c r="G22" t="s">
         <v>18</v>
       </c>
       <c r="H22">
         <f>B2*B5</f>
-        <v>54</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -799,7 +799,7 @@
       </c>
       <c r="H23">
         <f>B2*B5</f>
-        <v>54</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bugs with feedback
</commit_message>
<xml_diff>
--- a/Code/Overlap/RowCol calc.xlsx
+++ b/Code/Overlap/RowCol calc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Code\Overlap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4580CF07-10AC-4AE5-B3A9-4DB6E080819E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FD69ED-C919-4EB1-9203-D689A177F9C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F85780C8-78EB-42E2-BE9E-CEC15D110F12}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +464,7 @@
         <v>2</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -472,7 +472,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -480,7 +480,7 @@
         <v>15</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -497,7 +497,7 @@
       </c>
       <c r="B5">
         <f>B3+B4</f>
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -506,28 +506,28 @@
       </c>
       <c r="B11">
         <f>SUM(B12:B18)</f>
-        <v>2435</v>
+        <v>686</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E11">
         <f>SUM(E12:E18)</f>
-        <v>10430</v>
+        <v>3078</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H11">
         <f>SUM(H12:H17)</f>
-        <v>225</v>
+        <v>166</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="K11">
         <f>SUM(K12:K17)</f>
-        <v>1162</v>
+        <v>822</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -536,30 +536,30 @@
       </c>
       <c r="B12">
         <f>B2*B3</f>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D12">
         <f>B5</f>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E12">
         <f>B12*D12</f>
-        <v>196</v>
+        <v>144</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
       </c>
       <c r="H12">
         <f>B2</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J12">
         <f>B5</f>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="K12">
         <f t="shared" ref="K12:K17" si="0">H12*J12</f>
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -568,30 +568,30 @@
       </c>
       <c r="B13">
         <f>B2*B5</f>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D13">
         <f>B5</f>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E13">
         <f t="shared" ref="E13:E18" si="1">B13*D13</f>
-        <v>196</v>
+        <v>144</v>
       </c>
       <c r="G13" t="s">
         <v>7</v>
       </c>
       <c r="H13">
         <f>B2*B5</f>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="J13">
         <f>2+2*(B5-1)</f>
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>392</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -600,30 +600,30 @@
       </c>
       <c r="B14">
         <f>B2*(B3-1)</f>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D14">
         <f>2*B5</f>
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>364</v>
+        <v>240</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
       </c>
       <c r="H14">
         <f>B1*B3</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J14">
         <f>(B2/B1)*B5</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>196</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -632,29 +632,29 @@
       </c>
       <c r="B15">
         <f>B1*B3</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D15">
         <f>B2/B1 * B5</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>196</v>
+        <v>144</v>
       </c>
       <c r="G15" t="s">
         <v>9</v>
       </c>
       <c r="H15">
         <f>B2*B5*(B5-1)</f>
-        <v>182</v>
+        <v>120</v>
       </c>
       <c r="J15">
         <v>3</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>546</v>
+        <v>360</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -663,7 +663,7 @@
       </c>
       <c r="B16">
         <f>B2*B5*(B5-1)*(B5-1)</f>
-        <v>2366</v>
+        <v>600</v>
       </c>
       <c r="D16">
         <f>4</f>
@@ -671,21 +671,21 @@
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>9464</v>
+        <v>2400</v>
       </c>
       <c r="G16" t="s">
         <v>10</v>
       </c>
       <c r="H16">
         <f>B3</f>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J16">
         <v>1</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -694,14 +694,14 @@
       </c>
       <c r="B17">
         <f>B3</f>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>11</v>
@@ -712,7 +712,7 @@
       </c>
       <c r="J17">
         <f>B5</f>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
@@ -729,7 +729,7 @@
       </c>
       <c r="D18">
         <f>B5</f>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
@@ -742,7 +742,7 @@
       </c>
       <c r="H19">
         <f>H20+H21+H22+H23</f>
-        <v>224</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -751,14 +751,14 @@
       </c>
       <c r="B20">
         <f>B21+B22</f>
-        <v>210</v>
+        <v>150</v>
       </c>
       <c r="G20" t="s">
         <v>12</v>
       </c>
       <c r="H20">
         <f>B5</f>
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -767,14 +767,14 @@
       </c>
       <c r="B21">
         <f>B3</f>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G21" t="s">
         <v>13</v>
       </c>
       <c r="H21">
         <f>B2*B5*(B5-1)</f>
-        <v>182</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -783,14 +783,14 @@
       </c>
       <c r="B22">
         <f>B2*B3*B3</f>
-        <v>196</v>
+        <v>144</v>
       </c>
       <c r="G22" t="s">
         <v>18</v>
       </c>
       <c r="H22">
         <f>B2*B5</f>
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -799,7 +799,7 @@
       </c>
       <c r="H23">
         <f>B2*B5</f>
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added technicians to printed data, fixed issue in case rho==0
</commit_message>
<xml_diff>
--- a/Code/Overlap/RowCol calc.xlsx
+++ b/Code/Overlap/RowCol calc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Code\Overlap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08E5A87-18AD-4668-B31E-81DC67E08E4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE00CF1C-175E-4F64-B81C-06719C7BD55D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F85780C8-78EB-42E2-BE9E-CEC15D110F12}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{F85780C8-78EB-42E2-BE9E-CEC15D110F12}"/>
   </bookViews>
   <sheets>
     <sheet name="Year" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Rows</t>
   </si>
@@ -129,7 +129,31 @@
     <t>Maintenance 2</t>
   </si>
   <si>
-    <t>approx</t>
+    <t>Mp</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Resources P Up</t>
+  </si>
+  <si>
+    <t>Resources P Low</t>
+  </si>
+  <si>
+    <t>Resources R Low</t>
+  </si>
+  <si>
+    <t>Resources R Up</t>
+  </si>
+  <si>
+    <t>Deduction</t>
+  </si>
+  <si>
+    <t>approx based on M and gU</t>
+  </si>
+  <si>
+    <t>approx based on M and gL</t>
   </si>
 </sst>
 </file>
@@ -491,15 +515,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369586FE-FB47-484D-B8DA-5DFCD0818EDC}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:V29"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -507,7 +532,7 @@
         <v>2</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>27</v>
@@ -521,7 +546,7 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -535,7 +560,7 @@
         <v>18</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -543,7 +568,7 @@
         <v>19</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -559,15 +584,18 @@
         <v>0</v>
       </c>
       <c r="B11">
-        <f>SUM(B12:B16)</f>
-        <v>408</v>
+        <f>SUM(B12:B19)</f>
+        <v>23640</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E11">
-        <f>SUM(E12:E18)</f>
-        <v>2808</v>
+        <f>SUM(E12:E19)</f>
+        <v>362735</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="G11" s="1"/>
       <c r="J11" s="1"/>
@@ -578,138 +606,226 @@
       </c>
       <c r="B12">
         <f>B3*B2*B1</f>
-        <v>72</v>
+        <v>2400</v>
       </c>
       <c r="D12">
-        <f>1+B4+B5</f>
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="E12">
-        <f>B12*D12</f>
-        <v>648</v>
+        <f>B12*D12-F12</f>
+        <v>22800</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B13">
-        <f>B3*B2*B1</f>
-        <v>72</v>
+        <f>B2*B1</f>
+        <v>480</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="E13:E18" si="0">B13*D13</f>
-        <v>72</v>
+        <f t="shared" ref="E13:E19" si="0">B13*D13-F13</f>
+        <v>960</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B14">
-        <f>B3*B2*B5</f>
-        <v>120</v>
+        <f>B2*B1</f>
+        <v>480</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>360</v>
+        <v>3360</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B15">
-        <f>B4*B2</f>
-        <v>72</v>
+        <f>B1*B2*B5</f>
+        <v>2400</v>
       </c>
       <c r="D15">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>864</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
+        <v>4800</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B16">
+        <f>B1*B2*B3*B5</f>
+        <v>12000</v>
+      </c>
+      <c r="D16">
+        <v>1.5</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>18000</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <f>B3*B2*B5</f>
+        <v>3000</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>8975</v>
+      </c>
+      <c r="F17">
+        <f>B3*B5</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
         <f>B4*B2</f>
-        <v>72</v>
-      </c>
-      <c r="D16">
-        <v>12</v>
-      </c>
-      <c r="E16">
-        <f t="shared" ref="E16" si="1">B16*D16</f>
-        <v>864</v>
-      </c>
-      <c r="G16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <f>SUM(B19:B22)</f>
-        <v>384</v>
+        <v>1440</v>
+      </c>
+      <c r="D18">
+        <v>105.5</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>151920</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B19">
-        <f>B1*B2*B3</f>
-        <v>72</v>
-      </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20">
-        <f>B2*B4</f>
-        <v>72</v>
+        <f>B4*B2</f>
+        <v>1440</v>
+      </c>
+      <c r="D19">
+        <f>D18</f>
+        <v>105.5</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>151920</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>23</v>
+      <c r="A21" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B21">
-        <f>B2*B5*B3</f>
-        <v>120</v>
+        <f>SUM(B22:B27)</f>
+        <v>10800</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f>B1*B2</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f>B2*B4</f>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <f>B2*B5*B3</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B22">
+      <c r="B25">
         <f>B2*B5*B3</f>
-        <v>120</v>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26">
+        <f>B1*B2</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <f>B1*B2*B5</f>
+        <v>2400</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>